<commit_message>
merge files and and another fitter
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\floduR\Desktop\Kalibracia-Kamery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86B5B70-1EB1-4A2D-BB1F-F02FCB87FDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882AD86B-883A-488D-BA03-5453ABEA6E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1747,7 +1747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C9:DA150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S156" sqref="S156"/>
     </sheetView>
   </sheetViews>

</xml_diff>